<commit_message>
FeedBack upload Rating changes
</commit_message>
<xml_diff>
--- a/ytms-cli/src/assets/excel/FeedBack.xlsx
+++ b/ytms-cli/src/assets/excel/FeedBack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakash.sanap\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YTMSNEW\ytms-cli\ytms-cli\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C7482F-4004-4946-97D1-ADF5C829BFDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB60E2-C551-48C8-B54E-EF26BE92301D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{3808543F-ACB1-43E6-A90B-4CA520460CBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>Technical Skills</t>
+  </si>
+  <si>
+    <t>Attitude</t>
+  </si>
+  <si>
+    <t>Work Quality</t>
+  </si>
+  <si>
+    <t>Overall Rating</t>
+  </si>
+  <si>
+    <t>Communication Skills</t>
   </si>
 </sst>
 </file>
@@ -395,35 +410,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B089D3E-DDEB-4BEA-B320-1ACDC705A4EF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="27.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
         <v>3</v>
       </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>